<commit_message>
update file đánh giá
</commit_message>
<xml_diff>
--- a/report moi tuan/tuan 6/1159032-1359035-1359037-1359038.xlsx
+++ b/report moi tuan/tuan 6/1159032-1359035-1359037-1359038.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng quan" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
   <si>
     <t>MSSV</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t xml:space="preserve">project </t>
+  </si>
+  <si>
+    <t>Hoàn thành chức năng hiển thị sản phẩm và thông tin</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,6 +877,23 @@
         <v>46</v>
       </c>
     </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1359037</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -882,10 +902,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,6 +1304,23 @@
       </c>
       <c r="E23">
         <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="2">
+        <v>42649</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24">
+        <v>1359037</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>